<commit_message>
1st changes of mifos to finflux
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/2350-RBI-EI-DB-DL-REC-NOCOM-RNI-CTPD-DL-MD-TR-1-BLR-EARLY-CASH-Makerepayment1.xlsx
+++ b/Mifos Automation Excels/Client/2350-RBI-EI-DB-DL-REC-NOCOM-RNI-CTPD-DL-MD-TR-1-BLR-EARLY-CASH-Makerepayment1.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17766"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mifosx-e2e-testing\Mifos Automation Excels\Client\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="180" yWindow="495" windowWidth="15015" windowHeight="7620" tabRatio="439" activeTab="3"/>
+    <workbookView xWindow="180" yWindow="495" windowWidth="15015" windowHeight="7620" tabRatio="439" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="9" r:id="rId1"/>
@@ -115,7 +120,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -207,6 +212,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -254,7 +262,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -287,9 +295,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -322,6 +347,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -654,10 +696,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -673,11 +715,12 @@
     <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" customWidth="1"/>
+    <col min="15" max="15" width="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -715,16 +758,17 @@
       <c r="M1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="1"/>
+      <c r="O1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="1"/>
       <c r="P1" s="1"/>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="7">
@@ -750,8 +794,9 @@
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="P2" s="5"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -789,14 +834,15 @@
       <c r="M3" s="5">
         <v>0</v>
       </c>
-      <c r="N3" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="N3" s="5"/>
+      <c r="O3" s="5">
+        <v>0</v>
+      </c>
+      <c r="R3" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -832,14 +878,15 @@
       <c r="M4" s="5">
         <v>0</v>
       </c>
-      <c r="N4" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="5">
-        <v>846.75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="N4" s="5"/>
+      <c r="O4" s="5">
+        <v>0</v>
+      </c>
+      <c r="R4" s="5">
+        <v>846.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -875,14 +922,15 @@
       <c r="M5" s="5">
         <v>0</v>
       </c>
-      <c r="N5" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="5">
-        <v>846.75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="N5" s="5"/>
+      <c r="O5" s="5">
+        <v>0</v>
+      </c>
+      <c r="R5" s="5">
+        <v>846.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -918,14 +966,15 @@
       <c r="M6" s="5">
         <v>0</v>
       </c>
-      <c r="N6" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="5">
-        <v>846.75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="N6" s="5"/>
+      <c r="O6" s="5">
+        <v>0</v>
+      </c>
+      <c r="R6" s="5">
+        <v>846.75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -961,14 +1010,15 @@
       <c r="M7" s="5">
         <v>0</v>
       </c>
-      <c r="N7" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="5">
-        <v>846.75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="N7" s="5"/>
+      <c r="O7" s="5">
+        <v>0</v>
+      </c>
+      <c r="R7" s="5">
+        <v>846.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -1004,14 +1054,15 @@
       <c r="M8" s="5">
         <v>0</v>
       </c>
-      <c r="N8" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="5">
-        <v>846.75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="N8" s="5"/>
+      <c r="O8" s="5">
+        <v>0</v>
+      </c>
+      <c r="R8" s="5">
+        <v>846.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -1047,14 +1098,15 @@
       <c r="M9" s="5">
         <v>0</v>
       </c>
-      <c r="N9" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="5">
-        <v>846.75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="N9" s="5"/>
+      <c r="O9" s="5">
+        <v>0</v>
+      </c>
+      <c r="R9" s="5">
+        <v>846.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -1090,14 +1142,15 @@
       <c r="M10" s="5">
         <v>0</v>
       </c>
-      <c r="N10" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="5">
-        <v>846.75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="N10" s="5"/>
+      <c r="O10" s="5">
+        <v>0</v>
+      </c>
+      <c r="R10" s="5">
+        <v>846.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -1133,14 +1186,15 @@
       <c r="M11" s="5">
         <v>0</v>
       </c>
-      <c r="N11" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="5">
-        <v>846.75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="N11" s="5"/>
+      <c r="O11" s="5">
+        <v>0</v>
+      </c>
+      <c r="R11" s="5">
+        <v>846.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -1176,14 +1230,15 @@
       <c r="M12" s="5">
         <v>0</v>
       </c>
-      <c r="N12" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="5">
-        <v>846.75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="N12" s="5"/>
+      <c r="O12" s="5">
+        <v>0</v>
+      </c>
+      <c r="R12" s="5">
+        <v>846.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -1219,14 +1274,15 @@
       <c r="M13" s="5">
         <v>0</v>
       </c>
-      <c r="N13" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="5">
-        <v>846.75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="N13" s="5"/>
+      <c r="O13" s="5">
+        <v>0</v>
+      </c>
+      <c r="R13" s="5">
+        <v>846.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -1262,14 +1318,15 @@
       <c r="M14" s="5">
         <v>0</v>
       </c>
-      <c r="N14" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="5">
-        <v>846.75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="N14" s="5"/>
+      <c r="O14" s="5">
+        <v>0</v>
+      </c>
+      <c r="R14" s="5">
+        <v>846.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>13</v>
       </c>
@@ -1305,10 +1362,11 @@
       <c r="M15" s="5">
         <v>0</v>
       </c>
-      <c r="N15" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="5">
+      <c r="N15" s="5"/>
+      <c r="O15" s="5">
+        <v>0</v>
+      </c>
+      <c r="R15" s="5">
         <v>84.39</v>
       </c>
     </row>
@@ -1321,7 +1379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>

</xml_diff>